<commit_message>
Colour alterations for changed text.
</commit_message>
<xml_diff>
--- a/LCAM Documents/RevisedLCAMRiskList.xlsx
+++ b/LCAM Documents/RevisedLCAMRiskList.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\git\ITC303-9-Team1-Project\LCAM Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8E1EE9-2B3E-40FA-85C4-C68BE21ABA23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10BC7621-C4FF-45E0-AEB5-B7DFF167611F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="14880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1504,9 +1504,6 @@
     <t xml:space="preserve">Group members have demonstrated basic competency. However, depending on use case implementations complications can arise. </t>
   </si>
   <si>
-    <t xml:space="preserve">While allowing customisation such as font colour and size will be pleasing, it can cause unpredicted complications. </t>
-  </si>
-  <si>
     <t>As each use case will get implemented, group members might have different level of skills and  knowledge of the coding language which can cause complications. Therefore this remains as an open risk.</t>
   </si>
   <si>
@@ -1732,6 +1729,9 @@
   </si>
   <si>
     <t>15/6/23</t>
+  </si>
+  <si>
+    <t>While allowing customisation such as font colour and size will be pleasing, it can cause unpredicted complications. Final colour implementations are still being waited on</t>
   </si>
 </sst>
 </file>
@@ -1741,7 +1741,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1861,6 +1861,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -2318,7 +2324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2533,6 +2539,15 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="12" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2557,14 +2572,26 @@
     <xf numFmtId="49" fontId="18" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3051,11 +3078,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="74" t="str">
+      <c r="A1" s="77" t="str">
         <f>Risk_Tracking_Log!A1</f>
         <v>RISK MANAGEMENT LOG</v>
       </c>
-      <c r="B1" s="75"/>
+      <c r="B1" s="78"/>
     </row>
     <row r="2" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="63" t="s">
@@ -3231,9 +3258,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="112" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="112" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3414,7 +3441,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="111" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="76" t="s">
+      <c r="A7" s="79" t="s">
         <v>170</v>
       </c>
       <c r="B7" s="11" t="s">
@@ -3434,7 +3461,7 @@
         <v>81</v>
       </c>
       <c r="G7" s="73" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H7" s="37" t="s">
         <v>76</v>
@@ -3463,8 +3490,8 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="77"/>
-      <c r="B8" s="83" t="s">
+      <c r="A8" s="80"/>
+      <c r="B8" s="91" t="s">
         <v>97</v>
       </c>
       <c r="C8" s="22" t="s">
@@ -3506,8 +3533,8 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="77"/>
-      <c r="B9" s="11" t="s">
+      <c r="A9" s="80"/>
+      <c r="B9" s="91" t="s">
         <v>97</v>
       </c>
       <c r="C9" s="22" t="s">
@@ -3548,9 +3575,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="56.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="77"/>
-      <c r="B10" s="83" t="s">
+    <row r="10" spans="1:16" ht="45" x14ac:dyDescent="0.2">
+      <c r="A10" s="80"/>
+      <c r="B10" s="91" t="s">
         <v>97</v>
       </c>
       <c r="C10" s="22" t="s">
@@ -3592,9 +3619,9 @@
       </c>
       <c r="O10" s="64"/>
     </row>
-    <row r="11" spans="1:16" ht="67.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="77"/>
-      <c r="B11" s="83" t="s">
+    <row r="11" spans="1:16" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="80"/>
+      <c r="B11" s="91" t="s">
         <v>97</v>
       </c>
       <c r="C11" s="22" t="s">
@@ -3637,8 +3664,8 @@
       <c r="O11" s="64"/>
     </row>
     <row r="12" spans="1:16" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="77"/>
-      <c r="B12" s="11" t="s">
+      <c r="A12" s="80"/>
+      <c r="B12" s="75" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="22" t="s">
@@ -3654,8 +3681,8 @@
       <c r="F12" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="G12" s="67" t="s">
-        <v>193</v>
+      <c r="G12" s="88" t="s">
+        <v>192</v>
       </c>
       <c r="H12" s="36" t="s">
         <v>129</v>
@@ -3681,8 +3708,8 @@
       <c r="O12" s="64"/>
     </row>
     <row r="13" spans="1:16" ht="45" x14ac:dyDescent="0.2">
-      <c r="A13" s="78"/>
-      <c r="B13" s="83" t="s">
+      <c r="A13" s="81"/>
+      <c r="B13" s="91" t="s">
         <v>97</v>
       </c>
       <c r="C13" s="22" t="s">
@@ -3725,10 +3752,10 @@
       <c r="O13" s="64"/>
     </row>
     <row r="14" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="79" t="s">
+      <c r="A14" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="91" t="s">
         <v>97</v>
       </c>
       <c r="C14" s="22" t="s">
@@ -3771,8 +3798,8 @@
       <c r="O14" s="64"/>
     </row>
     <row r="15" spans="1:16" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="80"/>
-      <c r="B15" s="83" t="s">
+      <c r="A15" s="83"/>
+      <c r="B15" s="91" t="s">
         <v>97</v>
       </c>
       <c r="C15" s="22" t="s">
@@ -3814,9 +3841,9 @@
       </c>
       <c r="O15" s="64"/>
     </row>
-    <row r="16" spans="1:16" ht="67.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="80"/>
-      <c r="B16" s="83" t="s">
+    <row r="16" spans="1:16" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="83"/>
+      <c r="B16" s="75" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="22" t="s">
@@ -3832,8 +3859,8 @@
       <c r="F16" s="66" t="s">
         <v>152</v>
       </c>
-      <c r="G16" s="67" t="s">
-        <v>194</v>
+      <c r="G16" s="88" t="s">
+        <v>193</v>
       </c>
       <c r="H16" s="67" t="s">
         <v>153</v>
@@ -3859,7 +3886,7 @@
       <c r="O16" s="64"/>
     </row>
     <row r="17" spans="1:15" ht="45" x14ac:dyDescent="0.2">
-      <c r="A17" s="80"/>
+      <c r="A17" s="83"/>
       <c r="B17" s="11" t="s">
         <v>8</v>
       </c>
@@ -3876,8 +3903,8 @@
       <c r="F17" s="66" t="s">
         <v>165</v>
       </c>
-      <c r="G17" s="67" t="s">
-        <v>195</v>
+      <c r="G17" s="88" t="s">
+        <v>194</v>
       </c>
       <c r="H17" s="67" t="s">
         <v>146</v>
@@ -3903,7 +3930,7 @@
       <c r="O17" s="64"/>
     </row>
     <row r="18" spans="1:15" ht="56.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="80"/>
+      <c r="A18" s="83"/>
       <c r="B18" s="11" t="s">
         <v>8</v>
       </c>
@@ -3920,8 +3947,8 @@
       <c r="F18" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="G18" s="67" t="s">
-        <v>196</v>
+      <c r="G18" s="88" t="s">
+        <v>195</v>
       </c>
       <c r="H18" s="36" t="s">
         <v>134</v>
@@ -3946,8 +3973,8 @@
       </c>
       <c r="O18" s="64"/>
     </row>
-    <row r="19" spans="1:15" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="80"/>
+    <row r="19" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+      <c r="A19" s="83"/>
       <c r="B19" s="11" t="s">
         <v>8</v>
       </c>
@@ -3964,8 +3991,8 @@
       <c r="F19" s="66" t="s">
         <v>166</v>
       </c>
-      <c r="G19" s="67" t="s">
-        <v>180</v>
+      <c r="G19" s="88" t="s">
+        <v>255</v>
       </c>
       <c r="H19" s="67" t="s">
         <v>167</v>
@@ -3991,11 +4018,11 @@
       <c r="O19" s="64"/>
     </row>
     <row r="20" spans="1:15" ht="56.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="81"/>
+      <c r="A20" s="84"/>
       <c r="B20" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="82" t="s">
+      <c r="C20" s="74" t="s">
         <v>3</v>
       </c>
       <c r="D20" s="22" t="s">
@@ -4008,8 +4035,8 @@
       <c r="F20" s="66" t="s">
         <v>169</v>
       </c>
-      <c r="G20" s="67" t="s">
-        <v>197</v>
+      <c r="G20" s="88" t="s">
+        <v>196</v>
       </c>
       <c r="H20" s="36" t="s">
         <v>114</v>
@@ -4036,309 +4063,309 @@
     </row>
     <row r="21" spans="1:15" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A21" s="10"/>
-      <c r="B21" s="83" t="s">
+      <c r="B21" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="82" t="s">
+      <c r="C21" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="82" t="s">
+      <c r="D21" s="74" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="56" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
-      <c r="F21" s="66" t="s">
-        <v>182</v>
-      </c>
-      <c r="G21" s="67" t="s">
-        <v>192</v>
-      </c>
-      <c r="H21" s="67" t="s">
-        <v>205</v>
-      </c>
-      <c r="I21" s="67" t="s">
-        <v>213</v>
-      </c>
-      <c r="J21" s="68" t="s">
-        <v>224</v>
-      </c>
-      <c r="K21" s="67" t="s">
-        <v>226</v>
-      </c>
-      <c r="L21" s="70" t="s">
+      <c r="F21" s="87" t="s">
+        <v>181</v>
+      </c>
+      <c r="G21" s="88" t="s">
+        <v>191</v>
+      </c>
+      <c r="H21" s="88" t="s">
+        <v>204</v>
+      </c>
+      <c r="I21" s="88" t="s">
+        <v>212</v>
+      </c>
+      <c r="J21" s="89" t="s">
+        <v>223</v>
+      </c>
+      <c r="K21" s="88" t="s">
+        <v>225</v>
+      </c>
+      <c r="L21" s="90" t="s">
         <v>68</v>
       </c>
       <c r="M21" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="N21" s="69" t="s">
-        <v>218</v>
+      <c r="N21" s="85" t="s">
+        <v>217</v>
       </c>
       <c r="O21" s="64"/>
     </row>
-    <row r="22" spans="1:15" ht="67.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
-      <c r="B22" s="83" t="s">
+      <c r="B22" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="82" t="s">
+      <c r="C22" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="82" t="s">
+      <c r="D22" s="74" t="s">
         <v>1</v>
       </c>
       <c r="E22" s="56" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
-      <c r="F22" s="66" t="s">
-        <v>183</v>
-      </c>
-      <c r="G22" s="67" t="s">
-        <v>191</v>
-      </c>
-      <c r="H22" s="67" t="s">
-        <v>212</v>
-      </c>
-      <c r="I22" s="67" t="s">
+      <c r="F22" s="87" t="s">
+        <v>182</v>
+      </c>
+      <c r="G22" s="88" t="s">
+        <v>190</v>
+      </c>
+      <c r="H22" s="88" t="s">
+        <v>211</v>
+      </c>
+      <c r="I22" s="88" t="s">
         <v>141</v>
       </c>
-      <c r="J22" s="68" t="s">
-        <v>225</v>
-      </c>
-      <c r="K22" s="67" t="s">
-        <v>227</v>
-      </c>
-      <c r="L22" s="70" t="s">
+      <c r="J22" s="89" t="s">
+        <v>224</v>
+      </c>
+      <c r="K22" s="88" t="s">
+        <v>226</v>
+      </c>
+      <c r="L22" s="90" t="s">
         <v>68</v>
       </c>
       <c r="M22" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="N22" s="69" t="s">
-        <v>217</v>
+      <c r="N22" s="85" t="s">
+        <v>216</v>
       </c>
       <c r="O22" s="64"/>
     </row>
     <row r="23" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A23" s="10"/>
-      <c r="B23" s="83" t="s">
+      <c r="B23" s="91" t="s">
         <v>97</v>
       </c>
-      <c r="C23" s="82" t="s">
+      <c r="C23" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="82" t="s">
+      <c r="D23" s="74" t="s">
         <v>2</v>
       </c>
       <c r="E23" s="56" t="str">
         <f t="shared" si="0"/>
         <v>Closed</v>
       </c>
-      <c r="F23" s="66" t="s">
-        <v>184</v>
-      </c>
-      <c r="G23" s="67" t="s">
-        <v>200</v>
-      </c>
-      <c r="H23" s="67" t="s">
-        <v>206</v>
-      </c>
-      <c r="I23" s="67" t="s">
-        <v>214</v>
-      </c>
-      <c r="J23" s="68" t="s">
+      <c r="F23" s="87" t="s">
+        <v>183</v>
+      </c>
+      <c r="G23" s="88" t="s">
+        <v>199</v>
+      </c>
+      <c r="H23" s="88" t="s">
+        <v>205</v>
+      </c>
+      <c r="I23" s="88" t="s">
+        <v>213</v>
+      </c>
+      <c r="J23" s="89" t="s">
+        <v>227</v>
+      </c>
+      <c r="K23" s="88" t="s">
         <v>228</v>
       </c>
-      <c r="K23" s="67" t="s">
-        <v>229</v>
-      </c>
-      <c r="L23" s="70" t="s">
+      <c r="L23" s="90" t="s">
         <v>150</v>
       </c>
       <c r="M23" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="N23" s="69" t="s">
-        <v>219</v>
+      <c r="N23" s="85" t="s">
+        <v>218</v>
       </c>
       <c r="O23" s="64"/>
     </row>
     <row r="24" spans="1:15" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A24" s="10"/>
-      <c r="B24" s="83" t="s">
+      <c r="B24" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="82" t="s">
+      <c r="C24" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="82" t="s">
+      <c r="D24" s="74" t="s">
         <v>1</v>
       </c>
       <c r="E24" s="56" t="str">
         <f t="shared" si="0"/>
         <v>Red</v>
       </c>
-      <c r="F24" s="66" t="s">
-        <v>185</v>
-      </c>
-      <c r="G24" s="67" t="s">
-        <v>201</v>
-      </c>
-      <c r="H24" s="67" t="s">
-        <v>207</v>
-      </c>
-      <c r="I24" s="67" t="s">
-        <v>215</v>
-      </c>
-      <c r="J24" s="68" t="s">
+      <c r="F24" s="87" t="s">
+        <v>184</v>
+      </c>
+      <c r="G24" s="88" t="s">
+        <v>200</v>
+      </c>
+      <c r="H24" s="88" t="s">
+        <v>206</v>
+      </c>
+      <c r="I24" s="88" t="s">
+        <v>214</v>
+      </c>
+      <c r="J24" s="89" t="s">
+        <v>229</v>
+      </c>
+      <c r="K24" s="88" t="s">
         <v>230</v>
       </c>
-      <c r="K24" s="67" t="s">
-        <v>231</v>
-      </c>
-      <c r="L24" s="70" t="s">
+      <c r="L24" s="90" t="s">
         <v>68</v>
       </c>
       <c r="M24" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="N24" s="69" t="s">
-        <v>220</v>
+      <c r="N24" s="85" t="s">
+        <v>219</v>
       </c>
       <c r="O24" s="64"/>
     </row>
     <row r="25" spans="1:15" ht="67.5" x14ac:dyDescent="0.2">
       <c r="A25" s="10"/>
-      <c r="B25" s="83" t="s">
+      <c r="B25" s="91" t="s">
         <v>97</v>
       </c>
-      <c r="C25" s="82" t="s">
+      <c r="C25" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="82" t="s">
+      <c r="D25" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="E25" s="56" t="str">
+      <c r="E25" s="86" t="str">
         <f t="shared" si="0"/>
         <v>Closed</v>
       </c>
-      <c r="F25" s="66" t="s">
-        <v>186</v>
-      </c>
-      <c r="G25" s="67" t="s">
+      <c r="F25" s="87" t="s">
+        <v>185</v>
+      </c>
+      <c r="G25" s="88" t="s">
+        <v>207</v>
+      </c>
+      <c r="H25" s="88" t="s">
         <v>208</v>
       </c>
-      <c r="H25" s="67" t="s">
-        <v>209</v>
-      </c>
-      <c r="I25" s="67" t="s">
+      <c r="I25" s="88" t="s">
         <v>154</v>
       </c>
-      <c r="J25" s="68" t="s">
-        <v>235</v>
-      </c>
-      <c r="K25" s="67" t="s">
-        <v>232</v>
-      </c>
-      <c r="L25" s="70" t="s">
+      <c r="J25" s="89" t="s">
+        <v>234</v>
+      </c>
+      <c r="K25" s="88" t="s">
+        <v>231</v>
+      </c>
+      <c r="L25" s="90" t="s">
         <v>113</v>
       </c>
       <c r="M25" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="N25" s="69" t="s">
-        <v>221</v>
+      <c r="N25" s="85" t="s">
+        <v>220</v>
       </c>
       <c r="O25" s="64"/>
     </row>
     <row r="26" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
-      <c r="B26" s="83" t="s">
+      <c r="B26" s="91" t="s">
         <v>97</v>
       </c>
-      <c r="C26" s="82" t="s">
+      <c r="C26" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="82" t="s">
+      <c r="D26" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="E26" s="56" t="str">
+      <c r="E26" s="86" t="str">
         <f t="shared" si="0"/>
         <v>Closed</v>
       </c>
-      <c r="F26" s="66" t="s">
-        <v>188</v>
-      </c>
-      <c r="G26" s="67" t="s">
-        <v>202</v>
-      </c>
-      <c r="H26" s="67" t="s">
-        <v>210</v>
-      </c>
-      <c r="I26" s="67" t="s">
+      <c r="F26" s="87" t="s">
+        <v>187</v>
+      </c>
+      <c r="G26" s="88" t="s">
+        <v>201</v>
+      </c>
+      <c r="H26" s="88" t="s">
+        <v>209</v>
+      </c>
+      <c r="I26" s="88" t="s">
         <v>154</v>
       </c>
-      <c r="J26" s="68" t="s">
-        <v>237</v>
-      </c>
-      <c r="K26" s="67" t="s">
+      <c r="J26" s="89" t="s">
         <v>236</v>
       </c>
-      <c r="L26" s="70" t="s">
+      <c r="K26" s="88" t="s">
+        <v>235</v>
+      </c>
+      <c r="L26" s="90" t="s">
         <v>113</v>
       </c>
       <c r="M26" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="N26" s="69" t="s">
-        <v>222</v>
+      <c r="N26" s="85" t="s">
+        <v>221</v>
       </c>
       <c r="O26" s="64"/>
     </row>
     <row r="27" spans="1:15" ht="101.25" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
-      <c r="B27" s="83" t="s">
+      <c r="B27" s="91" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="82" t="s">
+      <c r="C27" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="82" t="s">
+      <c r="D27" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="56" t="str">
+      <c r="E27" s="86" t="str">
         <f t="shared" si="0"/>
         <v>Closed</v>
       </c>
-      <c r="F27" s="66" t="s">
-        <v>187</v>
-      </c>
-      <c r="G27" s="67" t="s">
-        <v>203</v>
-      </c>
-      <c r="H27" s="67" t="s">
-        <v>211</v>
-      </c>
-      <c r="I27" s="67" t="s">
-        <v>216</v>
-      </c>
-      <c r="J27" s="68" t="s">
-        <v>234</v>
-      </c>
-      <c r="K27" s="67" t="s">
+      <c r="F27" s="87" t="s">
+        <v>186</v>
+      </c>
+      <c r="G27" s="88" t="s">
+        <v>202</v>
+      </c>
+      <c r="H27" s="88" t="s">
+        <v>210</v>
+      </c>
+      <c r="I27" s="88" t="s">
+        <v>215</v>
+      </c>
+      <c r="J27" s="89" t="s">
         <v>233</v>
       </c>
-      <c r="L27" s="70" t="s">
+      <c r="K27" s="88" t="s">
+        <v>232</v>
+      </c>
+      <c r="L27" s="90" t="s">
         <v>150</v>
       </c>
       <c r="M27" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="N27" s="69" t="s">
-        <v>223</v>
+      <c r="N27" s="85" t="s">
+        <v>222</v>
       </c>
       <c r="O27" s="64"/>
     </row>
@@ -4424,14 +4451,14 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="N33" s="42" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O33" s="64"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B34" s="84"/>
-      <c r="C34" s="84"/>
-      <c r="D34" s="84"/>
+      <c r="B34" s="76"/>
+      <c r="C34" s="76"/>
+      <c r="D34" s="76"/>
       <c r="E34" s="42"/>
       <c r="J34" s="64"/>
       <c r="K34"/>
@@ -4440,10 +4467,10 @@
       <c r="N34"/>
     </row>
     <row r="35" spans="1:15" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="B35" s="84" t="s">
-        <v>189</v>
-      </c>
-      <c r="C35" s="84"/>
+      <c r="B35" s="76" t="s">
+        <v>188</v>
+      </c>
+      <c r="C35" s="76"/>
       <c r="D35" s="42"/>
       <c r="E35" s="42"/>
       <c r="F35" s="64"/>
@@ -4458,19 +4485,19 @@
     </row>
     <row r="36" spans="1:15" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="B36" s="84" t="s">
-        <v>245</v>
-      </c>
-      <c r="C36" s="84" t="s">
+        <v>197</v>
+      </c>
+      <c r="B36" s="76" t="s">
+        <v>244</v>
+      </c>
+      <c r="C36" s="76" t="s">
+        <v>246</v>
+      </c>
+      <c r="D36" s="76" t="s">
         <v>247</v>
       </c>
-      <c r="D36" s="84" t="s">
-        <v>248</v>
-      </c>
-      <c r="E36" s="84" t="s">
-        <v>250</v>
+      <c r="E36" s="76" t="s">
+        <v>249</v>
       </c>
       <c r="F36" s="64"/>
       <c r="G36"/>
@@ -4484,19 +4511,19 @@
     </row>
     <row r="37" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="B37" s="84" t="s">
-        <v>246</v>
-      </c>
-      <c r="C37" s="84" t="s">
-        <v>238</v>
-      </c>
-      <c r="D37" s="84" t="s">
-        <v>249</v>
-      </c>
-      <c r="E37" s="84" t="s">
-        <v>255</v>
+        <v>198</v>
+      </c>
+      <c r="B37" s="76" t="s">
+        <v>245</v>
+      </c>
+      <c r="C37" s="76" t="s">
+        <v>237</v>
+      </c>
+      <c r="D37" s="76" t="s">
+        <v>248</v>
+      </c>
+      <c r="E37" s="76" t="s">
+        <v>254</v>
       </c>
       <c r="G37" s="64"/>
       <c r="H37"/>
@@ -4508,17 +4535,17 @@
       <c r="N37"/>
     </row>
     <row r="38" spans="1:15" ht="45" x14ac:dyDescent="0.2">
-      <c r="B38" s="84" t="s">
-        <v>246</v>
-      </c>
-      <c r="C38" s="84" t="s">
-        <v>239</v>
-      </c>
-      <c r="D38" s="84" t="s">
-        <v>249</v>
-      </c>
-      <c r="E38" s="84" t="s">
-        <v>254</v>
+      <c r="B38" s="76" t="s">
+        <v>245</v>
+      </c>
+      <c r="C38" s="76" t="s">
+        <v>238</v>
+      </c>
+      <c r="D38" s="76" t="s">
+        <v>248</v>
+      </c>
+      <c r="E38" s="76" t="s">
+        <v>253</v>
       </c>
       <c r="G38" s="64"/>
       <c r="H38"/>
@@ -4530,17 +4557,17 @@
       <c r="N38"/>
     </row>
     <row r="39" spans="1:15" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="B39" s="84" t="s">
-        <v>190</v>
-      </c>
-      <c r="C39" s="84" t="s">
-        <v>241</v>
-      </c>
-      <c r="D39" s="84" t="s">
-        <v>249</v>
-      </c>
-      <c r="E39" s="84" t="s">
-        <v>254</v>
+      <c r="B39" s="76" t="s">
+        <v>189</v>
+      </c>
+      <c r="C39" s="76" t="s">
+        <v>240</v>
+      </c>
+      <c r="D39" s="76" t="s">
+        <v>248</v>
+      </c>
+      <c r="E39" s="76" t="s">
+        <v>253</v>
       </c>
       <c r="G39" s="64"/>
       <c r="H39"/>
@@ -4552,76 +4579,76 @@
       <c r="N39"/>
     </row>
     <row r="40" spans="1:15" ht="45" x14ac:dyDescent="0.2">
-      <c r="B40" s="84" t="s">
-        <v>246</v>
-      </c>
-      <c r="C40" s="84" t="s">
-        <v>240</v>
-      </c>
-      <c r="D40" s="84" t="s">
-        <v>249</v>
-      </c>
-      <c r="E40" s="84" t="s">
-        <v>253</v>
+      <c r="B40" s="76" t="s">
+        <v>245</v>
+      </c>
+      <c r="C40" s="76" t="s">
+        <v>239</v>
+      </c>
+      <c r="D40" s="76" t="s">
+        <v>248</v>
+      </c>
+      <c r="E40" s="76" t="s">
+        <v>252</v>
       </c>
       <c r="L40" s="64"/>
       <c r="M40"/>
       <c r="N40"/>
     </row>
     <row r="41" spans="1:15" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="B41" s="84" t="s">
-        <v>190</v>
-      </c>
-      <c r="C41" s="84" t="s">
-        <v>242</v>
-      </c>
-      <c r="D41" s="84" t="s">
-        <v>249</v>
-      </c>
-      <c r="E41" s="84" t="s">
-        <v>253</v>
+      <c r="B41" s="76" t="s">
+        <v>189</v>
+      </c>
+      <c r="C41" s="76" t="s">
+        <v>241</v>
+      </c>
+      <c r="D41" s="76" t="s">
+        <v>248</v>
+      </c>
+      <c r="E41" s="76" t="s">
+        <v>252</v>
       </c>
       <c r="L41" s="64"/>
       <c r="M41"/>
       <c r="N41"/>
     </row>
     <row r="42" spans="1:15" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="B42" s="84" t="s">
-        <v>190</v>
-      </c>
-      <c r="C42" s="84" t="s">
-        <v>243</v>
-      </c>
-      <c r="D42" s="84" t="s">
-        <v>249</v>
-      </c>
-      <c r="E42" s="84" t="s">
-        <v>252</v>
+      <c r="B42" s="76" t="s">
+        <v>189</v>
+      </c>
+      <c r="C42" s="76" t="s">
+        <v>242</v>
+      </c>
+      <c r="D42" s="76" t="s">
+        <v>248</v>
+      </c>
+      <c r="E42" s="76" t="s">
+        <v>251</v>
       </c>
       <c r="L42" s="64"/>
       <c r="M42"/>
       <c r="N42"/>
     </row>
     <row r="43" spans="1:15" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="B43" s="84" t="s">
-        <v>190</v>
-      </c>
-      <c r="C43" s="84" t="s">
-        <v>244</v>
-      </c>
-      <c r="D43" s="84" t="s">
-        <v>249</v>
-      </c>
-      <c r="E43" s="84" t="s">
-        <v>251</v>
+      <c r="B43" s="76" t="s">
+        <v>189</v>
+      </c>
+      <c r="C43" s="76" t="s">
+        <v>243</v>
+      </c>
+      <c r="D43" s="76" t="s">
+        <v>248</v>
+      </c>
+      <c r="E43" s="76" t="s">
+        <v>250</v>
       </c>
       <c r="L43" s="64"/>
       <c r="M43"/>
       <c r="N43"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B44" s="84"/>
-      <c r="C44" s="84"/>
+      <c r="B44" s="76"/>
+      <c r="C44" s="76"/>
       <c r="D44" s="42"/>
       <c r="E44" s="42"/>
       <c r="L44" s="64"/>
@@ -4629,8 +4656,8 @@
       <c r="N44"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B45" s="84"/>
-      <c r="C45" s="84"/>
+      <c r="B45" s="76"/>
+      <c r="C45" s="76"/>
       <c r="D45" s="42"/>
       <c r="E45" s="42"/>
       <c r="L45" s="64"/>
@@ -4638,8 +4665,8 @@
       <c r="N45"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B46" s="84"/>
-      <c r="C46" s="84"/>
+      <c r="B46" s="76"/>
+      <c r="C46" s="76"/>
       <c r="D46" s="42"/>
       <c r="E46" s="42"/>
       <c r="L46" s="64"/>
@@ -4647,8 +4674,8 @@
       <c r="N46"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B47" s="84"/>
-      <c r="C47" s="84"/>
+      <c r="B47" s="76"/>
+      <c r="C47" s="76"/>
       <c r="D47" s="42"/>
       <c r="E47" s="42"/>
       <c r="L47" s="64"/>
@@ -4656,8 +4683,8 @@
       <c r="N47"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B48" s="84"/>
-      <c r="C48" s="84"/>
+      <c r="B48" s="76"/>
+      <c r="C48" s="76"/>
       <c r="D48" s="42"/>
       <c r="E48" s="42"/>
       <c r="L48" s="64"/>
@@ -4907,7 +4934,7 @@
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:E1 B6:C6 B7:B27 C33:E33 C50:C65526 D50:E65525 B39:B48">
+  <conditionalFormatting sqref="C1:E1 B6:C6 B7:B27 C33:E33 B39:B48 D50:E65525 C50:C65526">
     <cfRule type="cellIs" dxfId="7" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>

</xml_diff>